<commit_message>
Updated WPs and Mobility
</commit_message>
<xml_diff>
--- a/fa_ansokan_forskardoktor_sv_ovriga_sep2016.xlsx
+++ b/fa_ansokan_forskardoktor_sv_ovriga_sep2016.xlsx
@@ -1516,9 +1516,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>645840</xdr:colOff>
+      <xdr:colOff>645480</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1531,8 +1531,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7762680" y="142920"/>
-          <a:ext cx="417240" cy="342000"/>
+          <a:off x="8278200" y="142920"/>
+          <a:ext cx="416880" cy="341640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1553,9 +1553,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>897120</xdr:colOff>
+      <xdr:colOff>896760</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>151920</xdr:rowOff>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1568,8 +1568,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="249480" y="114480"/>
-          <a:ext cx="1146600" cy="1218240"/>
+          <a:off x="269640" y="114480"/>
+          <a:ext cx="1166760" cy="1217880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1590,9 +1590,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>237600</xdr:colOff>
+      <xdr:colOff>237240</xdr:colOff>
       <xdr:row>66</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1602,7 +1602,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10734120" cy="9524520"/>
+          <a:ext cx="11476440" cy="9524160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1640,9 +1640,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>455760</xdr:colOff>
+      <xdr:colOff>455400</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1655,8 +1655,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="663480" y="57240"/>
-          <a:ext cx="1081080" cy="1142280"/>
+          <a:off x="714960" y="57240"/>
+          <a:ext cx="1132200" cy="1141920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1678,33 +1678,32 @@
   </sheetPr>
   <dimension ref="A1:W74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V22" activeCellId="0" sqref="V22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W12" activeCellId="0" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="3.53571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.4030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="3.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.8775510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="0.88265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.06632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="6.62244897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.51530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="7.06632653061225"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="0.88265306122449"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.04081632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="6.33673469387755"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="0.88265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.1938775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.53571428571429"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.1938775510204"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.53571428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.1938775510204"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.53571428571429"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.1938775510204"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="3.53571428571429"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.8979591836735"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="3.53571428571429"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9234693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="3.8265306122449"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.9234693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="3.8265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.9234693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="3.8265306122449"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.9234693877551"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="3.8265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.6377551020408"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="3.8265306122449"/>
     <col collapsed="false" hidden="true" max="21" min="20" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="9.28061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="9.13265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="9.86224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1924,7 +1923,7 @@
       <c r="R9" s="10"/>
       <c r="S9" s="9"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
@@ -1935,19 +1934,19 @@
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="19" t="n">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="K10" s="6"/>
       <c r="L10" s="19" t="n">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="19" t="n">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="O10" s="6"/>
       <c r="P10" s="19" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="Q10" s="6"/>
       <c r="R10" s="20" t="s">
@@ -2943,22 +2942,22 @@
       <c r="I41" s="6"/>
       <c r="J41" s="81" t="n">
         <f aca="false">J10</f>
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="K41" s="6"/>
       <c r="L41" s="81" t="n">
         <f aca="false">L10</f>
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="M41" s="6"/>
       <c r="N41" s="81" t="n">
         <f aca="false">N10</f>
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="O41" s="6"/>
       <c r="P41" s="81" t="n">
         <f aca="false">P10</f>
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="Q41" s="6"/>
       <c r="R41" s="20" t="s">
@@ -3958,11 +3957,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.13265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.28061224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.13265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.86224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="9.86224489795918"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="0.88265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.13265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="9.86224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>